<commit_message>
Fix columns and their content:date, time, genre. Splitted the date and time. Changed dramatic to drama, dollhouse to puppet show in Russian language
</commit_message>
<xml_diff>
--- a/all_performance_dict.xlsx
+++ b/all_performance_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>День и время:</t>
+          <t>Дата:</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Время:</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Жанр:</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Рейтинг:</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Цена:</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Театр:</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Описание:</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>URL спектакля:</t>
         </is>
@@ -486,33 +491,38 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1 апреля в 19:00</t>
+          <t>1 апреля</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>7.4</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>От 1000 ₽</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>ДК им. Ленсовета</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Виктор Сухоруков в трогательной комедии Вампилова</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/90900/</t>
         </is>
@@ -529,33 +539,38 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10 апреля в 18:00</t>
+          <t>10 апреля</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Перформанс</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>7.8</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>От 900 ₽</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Скороход</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Щекотливый спектакль без актеров и декораций</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/118145/</t>
         </is>
@@ -567,40 +582,45 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Враки, или Завещание барона Мюнхгаузена</t>
+          <t>Смешанные чувства</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25 марта в 19:00</t>
+          <t>24 марта</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Премьеры</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>От 6500 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>7.1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>От 400 ₽</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Константин Хабенский в роли легендарного барона</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/245895/</t>
+          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/79983/</t>
         </is>
       </c>
     </row>
@@ -610,40 +630,45 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Иисус Христос — суперзвезда</t>
+          <t>Враки, или Завещание барона Мюнхгаузена</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>24 апреля в 19:00</t>
+          <t>25 марта</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Музыкальный</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Премьеры</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>6.3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>От 6500 ₽</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Постановка питерского театра «Рок-опера»</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/66149/</t>
+          <t>Константин Хабенский в роли легендарного барона</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/245895/</t>
         </is>
       </c>
     </row>
@@ -653,40 +678,45 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Город. Женитьба. Гоголь</t>
+          <t>Иисус Христос — суперзвезда</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>29 апреля в 19:00</t>
+          <t>24 апреля</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>От 600 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Музыкальный</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>8.5</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Герои Гоголя растворяются в современном Петербурге</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/103390/</t>
+          <t>Постановка питерского театра «Рок-опера»</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/66149/</t>
         </is>
       </c>
     </row>
@@ -696,40 +726,45 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Смешанные чувства</t>
+          <t>Валентинов день</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24 марта в 19:00</t>
+          <t>3 апреля</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Комедия</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>От 600 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>7.4</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 700 ₽</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/79983/</t>
+          <t>Иван Вырыпаев в антрепризе</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/88299/</t>
         </is>
       </c>
     </row>
@@ -739,40 +774,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Валентинов день</t>
+          <t>Город. Женитьба. Гоголь</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3 апреля в 19:00</t>
+          <t>29 апреля</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>От 700 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>8.199999999999999</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>От 600 ₽</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Иван Вырыпаев в антрепризе</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/88299/</t>
+          <t>Герои Гоголя растворяются в современном Петербурге</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/103390/</t>
         </is>
       </c>
     </row>
@@ -782,40 +822,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Все мы прекрасные люди</t>
+          <t>Ревизор</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>19 апреля в 19:00</t>
+          <t>27 марта</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Комедия</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>От 400 ₽</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Театр им. Ленсовета</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/96366/</t>
+          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/78711/</t>
         </is>
       </c>
     </row>
@@ -825,40 +870,45 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>С Чарльзом Буковски за барной стойкой</t>
+          <t>Все мы прекрасные люди</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Завтра в 19:00</t>
+          <t>19 апреля</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Перформанс</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>От 900 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>4.5</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Fiddler's Green</t>
+          <t>От 400 ₽</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/191308/</t>
+          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/96366/</t>
         </is>
       </c>
     </row>
@@ -868,40 +918,45 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Топливо</t>
+          <t>Гроза</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>31 марта в 20:00</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>8</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Увлекательный байопик про российского физика</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/104731/</t>
+          <t>Большое шаманство Андрея Могучего по Островскому</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/117877/</t>
         </is>
       </c>
     </row>
@@ -911,40 +966,45 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ревизор</t>
+          <t>Топливо</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>27 марта в 19:00</t>
+          <t>31 марта</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Комедия</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>8.4</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/78711/</t>
+          <t>Увлекательный байопик про российского физика</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/104731/</t>
         </is>
       </c>
     </row>
@@ -954,40 +1014,45 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Когда я снова стану маленьким</t>
+          <t>Записки юного врача</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3 апреля в 13:00</t>
+          <t>2 апреля</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Кукольный</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Билеты</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>7.7</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>От 700 ₽</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
+          <t>Мастерская</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/97786/</t>
+          <t>Моноспектакль по ранним рассказам Булгакова</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/117716/</t>
         </is>
       </c>
     </row>
@@ -997,40 +1062,45 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Гроза</t>
+          <t>С Чарльзом Буковски за барной стойкой</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>20 марта в 18:00</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>8</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Перформанс</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>5.2</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>От 900 ₽</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Большое шаманство Андрея Могучего по Островскому</t>
+          <t>Fiddler's Green</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117877/</t>
+          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/191308/</t>
         </is>
       </c>
     </row>
@@ -1040,40 +1110,45 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Скамейка</t>
+          <t>Преступление и наказание</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6 апреля в 19:00</t>
+          <t>24 марта</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>От 500 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>8.699999999999999</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Концертный зал в здании Екатерининского собрания</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Не самая банальная советская мелодрама, сыгранная как французский шансон</t>
+          <t>Небольшой драматический театр</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/77005/</t>
+          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/90576/</t>
         </is>
       </c>
     </row>
@@ -1083,40 +1158,45 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Буря</t>
+          <t>Безымянная звезда</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3 апреля в 19:00</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="F16" t="inlineStr">
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>От 300 ₽</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Умный трагифарс от режиссера Морфова, фокусы с пространством от художника Капелюша</t>
-        </is>
-      </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/65972/</t>
+          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/67513/</t>
         </is>
       </c>
     </row>
@@ -1126,40 +1206,45 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Преступление и наказание</t>
+          <t>Дети солнца</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>24 марта в 19:00</t>
+          <t>23 апреля</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>6.6</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Небольшой драматический театр</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/90576/</t>
+          <t>Размышления об идеальном человеке</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/233405/</t>
         </is>
       </c>
     </row>
@@ -1169,40 +1254,45 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Сон об осени</t>
+          <t>Когда я снова стану маленьким</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Завтра в 19:00</t>
+          <t>8 апреля</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Кукольный спектакль</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>8.300000000000001</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 2000 ₽</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Современная норвежская пьеса про жизнь как ожидание чуда</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/115932/</t>
+          <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/97786/</t>
         </is>
       </c>
     </row>
@@ -1212,40 +1302,45 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Безымянная звезда</t>
+          <t>Что делать</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>20 марта в 19:00</t>
+          <t>29 марта</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>6.2</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>От 500 ₽</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67513/</t>
+          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/101454/</t>
         </is>
       </c>
     </row>
@@ -1260,33 +1355,38 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9 апреля в 19:00</t>
+          <t>9 апреля</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>8.6</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>От 500 ₽</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>БДТ</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/190192/</t>
         </is>
@@ -1298,40 +1398,45 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Что делать</t>
+          <t>Дон Жуан</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>29 марта в 19:00</t>
+          <t>17 апреля</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>От 500 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>6.9</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+          <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/101454/</t>
+          <t>История про «эпикурейскую свинью», которой, однако, есть, что сказать и донне Анне и Создателю</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/67156/</t>
         </is>
       </c>
     </row>
@@ -1346,33 +1451,38 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>20 марта в 14:00</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>8.5</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>От 2500 ₽</t>
-        </is>
-      </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>От 1000 ₽</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>Мастерская</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>Восьмичасовой спектакль о казаках</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/94169/</t>
         </is>
@@ -1389,33 +1499,38 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>18 марта в 19:00</t>
+          <t>30 апреля</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>7.7</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>От 1900 ₽</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
+          <t>От 700 ₽</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
           <t>Мастерская</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Обаятельный иллюстративный спектакль по пьесе Вампилова</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/83020/</t>
         </is>
@@ -1427,81 +1542,43 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Дон Жуан</t>
+          <t>Трамвай «Желание»</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>19 марта в 19:00</t>
+          <t>7 апреля</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>7.3</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>История про «эпикурейскую свинью», которой, однако, есть, что сказать и донне Анне и Создателю</t>
+          <t>Приют комедианта</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67156/</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Трамвай «Желание»</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>7 апреля в 19:00</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Драматический</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Приют комедианта</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
           <t>Жестокая мелодрама с хорошими актерами</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/68360/</t>
         </is>

</xml_diff>

<commit_message>
Gitignore private file, add columns in parsing table
</commit_message>
<xml_diff>
--- a/all_performance_dict.xlsx
+++ b/all_performance_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,47 +436,52 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Название спектакля:</t>
+          <t>Название спектакля</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Дата:</t>
+          <t>Дата</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Время:</t>
+          <t>Время</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Жанр:</t>
+          <t>Жанр</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Рейтинг:</t>
+          <t>Возраст</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Цена:</t>
+          <t>Рейтинг</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Театр:</t>
+          <t>Цена</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Описание:</t>
+          <t>Театр</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>URL спектакля:</t>
+          <t>Описание</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>URL спектакля</t>
         </is>
       </c>
     </row>
@@ -504,25 +509,30 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>7.4</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>От 1000 ₽</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>ДК им. Ленсовета</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Виктор Сухоруков в трогательной комедии Вампилова</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/90900/</t>
         </is>
@@ -552,25 +562,30 @@
           <t>Перформанс</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>7.8</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>От 900 ₽</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Скороход</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Щекотливый спектакль без актеров и декораций</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/118145/</t>
         </is>
@@ -587,7 +602,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24 марта</t>
+          <t>21 апреля</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -600,25 +615,30 @@
           <t>Комедия</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>7.1</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>От 400 ₽</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Театр им. Ленсовета</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/79983/</t>
         </is>
@@ -648,25 +668,30 @@
           <t>Премьеры</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>6.3</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>От 6500 ₽</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>От 9000 ₽</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>Александринский театр</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Константин Хабенский в роли легендарного барона</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/245895/</t>
         </is>
@@ -678,12 +703,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Иисус Христос — суперзвезда</t>
+          <t>Валентинов день</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>24 апреля</t>
+          <t>3 апреля</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -693,30 +718,35 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Музыкальный</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>7.4</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>От 700 ₽</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>ДК им. Ленсовета</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Постановка питерского театра «Рок-опера»</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/66149/</t>
+          <t>Иван Вырыпаев в антрепризе</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/88299/</t>
         </is>
       </c>
     </row>
@@ -726,12 +756,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Валентинов день</t>
+          <t>Иисус Христос — суперзвезда</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3 апреля</t>
+          <t>24 апреля</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -741,30 +771,35 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Драма</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>От 700 ₽</t>
-        </is>
+          <t>Музыкальный</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>8.5</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>От 1000 ₽</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>ДК им. Ленсовета</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Иван Вырыпаев в антрепризе</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/88299/</t>
+          <t>Постановка питерского театра «Рок-опера»</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/66149/</t>
         </is>
       </c>
     </row>
@@ -774,12 +809,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Город. Женитьба. Гоголь</t>
+          <t>Записки юного врача</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>29 апреля</t>
+          <t>2 апреля</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -792,27 +827,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>От 600 ₽</t>
-        </is>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>7.7</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 1200 ₽</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Герои Гоголя растворяются в современном Петербурге</t>
+          <t>Мастерская</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/103390/</t>
+          <t>Моноспектакль по ранним рассказам Булгакова</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/117716/</t>
         </is>
       </c>
     </row>
@@ -822,45 +862,50 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ревизор</t>
+          <t>Топливо</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>27 марта</t>
+          <t>31 марта</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Комедия</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>8.4</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/78711/</t>
+          <t>Увлекательный байопик про российского физика</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/104731/</t>
         </is>
       </c>
     </row>
@@ -870,12 +915,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Все мы прекрасные люди</t>
+          <t>Гроза</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>19 апреля</t>
+          <t>28 апреля</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -885,30 +930,35 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Комедия</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/96366/</t>
+          <t>Большое шаманство Андрея Могучего по Островскому</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/117877/</t>
         </is>
       </c>
     </row>
@@ -918,45 +968,50 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Гроза</t>
+          <t>Ревизор</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Сегодня</t>
+          <t>26 июня</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Драма</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>8</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>8.1</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>От 400 ₽</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Большое шаманство Андрея Могучего по Островскому</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117877/</t>
+          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/78711/</t>
         </is>
       </c>
     </row>
@@ -966,45 +1021,50 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Топливо</t>
+          <t>С Чарльзом Буковски за барной стойкой</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>31 марта</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Драма</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>Перформанс</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>5.2</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>От 900 ₽</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Увлекательный байопик про российского физика</t>
+          <t>Fiddler's Green</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/104731/</t>
+          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/191308/</t>
         </is>
       </c>
     </row>
@@ -1014,12 +1074,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Записки юного врача</t>
+          <t>Безымянная звезда</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2 апреля</t>
+          <t>7 апреля</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1032,27 +1092,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>От 700 ₽</t>
-        </is>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>14+</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>8.199999999999999</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Мастерская</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Моноспектакль по ранним рассказам Булгакова</t>
+          <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117716/</t>
+          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/67513/</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1127,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>С Чарльзом Буковски за барной стойкой</t>
+          <t>Город. Женитьба. Гоголь</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Сегодня</t>
+          <t>29 апреля</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1077,30 +1142,35 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Перформанс</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>От 900 ₽</t>
-        </is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>8.199999999999999</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Fiddler's Green</t>
+          <t>От 600 ₽</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/191308/</t>
+          <t>Герои Гоголя растворяются в современном Петербурге</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/103390/</t>
         </is>
       </c>
     </row>
@@ -1110,12 +1180,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Преступление и наказание</t>
+          <t>Лето одного года</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24 марта</t>
+          <t>8 апреля</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1128,27 +1198,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>8.9</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Небольшой драматический театр</t>
+          <t>От 4000 ₽</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/90576/</t>
+          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/82546/</t>
         </is>
       </c>
     </row>
@@ -1158,12 +1233,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Безымянная звезда</t>
+          <t>Дети солнца</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Сегодня</t>
+          <t>23 апреля</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1176,27 +1251,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>От 4000 ₽</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67513/</t>
+          <t>Размышления об идеальном человеке</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/233405/</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1286,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Дети солнца</t>
+          <t>Преступление и наказание</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>23 апреля</t>
+          <t>29 апреля</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1224,27 +1304,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>8.699999999999999</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Размышления об идеальном человеке</t>
+          <t>Небольшой драматический театр</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/233405/</t>
+          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/90576/</t>
         </is>
       </c>
     </row>
@@ -1259,12 +1344,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8 апреля</t>
+          <t>24 апреля</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1272,25 +1357,30 @@
           <t>Кукольный спектакль</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>6+</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>От 2000 ₽</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>Билеты</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>БДТ</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/97786/</t>
         </is>
@@ -1320,25 +1410,30 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
         <v>6.2</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>От 500 ₽</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>БДТ</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/101454/</t>
         </is>
@@ -1350,12 +1445,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Губернатор</t>
+          <t>Все мы прекрасные люди</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9 апреля</t>
+          <t>19 апреля</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1365,30 +1460,35 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Драма</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>От 500 ₽</t>
-        </is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>4.5</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>От 600 ₽</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/190192/</t>
+          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/96366/</t>
         </is>
       </c>
     </row>
@@ -1398,12 +1498,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Дон Жуан</t>
+          <t>Губернатор</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>17 апреля</t>
+          <t>9 апреля</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1416,27 +1516,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>8.6</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>От 500 ₽</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>История про «эпикурейскую свинью», которой, однако, есть, что сказать и донне Анне и Создателю</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67156/</t>
+          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/190192/</t>
         </is>
       </c>
     </row>
@@ -1446,17 +1551,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Тихий Дон. Истоки. Берега</t>
+          <t>Билли Миллиган</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Сегодня</t>
+          <t>18 апреля</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1464,27 +1569,32 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>5.2</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Мастерская</t>
+          <t>От 1200 ₽</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Восьмичасовой спектакль о казаках</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/94169/</t>
+          <t>Триллер про самого известного психа в истории</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/118241/</t>
         </is>
       </c>
     </row>
@@ -1494,12 +1604,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Старший сын</t>
+          <t>Трамвай «Желание»</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>30 апреля</t>
+          <t>7 апреля</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1512,73 +1622,30 @@
           <t>Драма</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>От 700 ₽</t>
-        </is>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>7.3</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Мастерская</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Обаятельный иллюстративный спектакль по пьесе Вампилова</t>
+          <t>Приют комедианта</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/83020/</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Трамвай «Желание»</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>7 апреля</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Драма</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Приют комедианта</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
           <t>Жестокая мелодрама с хорошими актерами</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>https://www.afisha.ru/performance/68360/</t>
         </is>

</xml_diff>

<commit_message>
Return to normal version with gitignore
</commit_message>
<xml_diff>
--- a/all_performance_dict.xlsx
+++ b/all_performance_dict.xlsx
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>От 9000 ₽</t>
+          <t>От 400 ₽</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -862,22 +862,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Топливо</t>
+          <t>Ревизор</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>31 марта</t>
+          <t>26 июня</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -886,26 +886,26 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>От 1000 ₽</t>
+          <t>От 400 ₽</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Увлекательный байопик про российского физика</t>
+          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/104731/</t>
+          <t>https://www.afisha.ru/performance/78711/</t>
         </is>
       </c>
     </row>
@@ -915,12 +915,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Гроза</t>
+          <t>Лето одного года</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>28 апреля</t>
+          <t>8 апреля</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -935,15 +935,15 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>16+</t>
+          <t>12+</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>8</v>
+        <v>8.9</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>От 300 ₽</t>
+          <t>От 4000 ₽</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -953,12 +953,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Большое шаманство Андрея Могучего по Островскому</t>
+          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117877/</t>
+          <t>https://www.afisha.ru/performance/82546/</t>
         </is>
       </c>
     </row>
@@ -968,22 +968,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ревизор</t>
+          <t>Топливо</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>26 июня</t>
+          <t>31 марта</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -992,26 +992,26 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8.1</v>
+        <v>8.4</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>От 400 ₽</t>
+          <t>От 1000 ₽</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+          <t>Увлекательный байопик про российского физика</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/78711/</t>
+          <t>https://www.afisha.ru/performance/104731/</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>С Чарльзом Буковски за барной стойкой</t>
+          <t>Гроза</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Сегодня</t>
+          <t>28 апреля</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1036,35 +1036,35 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Перформанс</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>18+</t>
+          <t>16+</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>5.2</v>
+        <v>8</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>От 900 ₽</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Fiddler's Green</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+          <t>Большое шаманство Андрея Могучего по Островскому</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/191308/</t>
+          <t>https://www.afisha.ru/performance/117877/</t>
         </is>
       </c>
     </row>
@@ -1074,12 +1074,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Безымянная звезда</t>
+          <t>С Чарльзом Буковски за барной стойкой</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7 апреля</t>
+          <t>Сегодня</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1089,35 +1089,35 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Перформанс</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>14+</t>
+          <t>18+</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>8.199999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>От 300 ₽</t>
+          <t>От 900 ₽</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>Fiddler's Green</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67513/</t>
+          <t>https://www.afisha.ru/performance/191308/</t>
         </is>
       </c>
     </row>
@@ -1127,12 +1127,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Город. Женитьба. Гоголь</t>
+          <t>Безымянная звезда</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>29 апреля</t>
+          <t>7 апреля</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>12+</t>
+          <t>14+</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1155,22 +1155,22 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>От 600 ₽</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Герои Гоголя растворяются в современном Петербурге</t>
+          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/103390/</t>
+          <t>https://www.afisha.ru/performance/67513/</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Лето одного года</t>
+          <t>Дети солнца</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8 апреля</t>
+          <t>23 апреля</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1200,30 +1200,30 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>12+</t>
+          <t>16+</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>8.9</v>
+        <v>5</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>От 4000 ₽</t>
+          <t>От 300 ₽</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
+          <t>Размышления об идеальном человеке</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/82546/</t>
+          <t>https://www.afisha.ru/performance/233405/</t>
         </is>
       </c>
     </row>
@@ -1233,12 +1233,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Дети солнца</t>
+          <t>Что делать</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>23 апреля</t>
+          <t>29 марта</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1257,26 +1257,26 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>От 4000 ₽</t>
+          <t>От 500 ₽</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Размышления об идеальном человеке</t>
+          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/233405/</t>
+          <t>https://www.afisha.ru/performance/101454/</t>
         </is>
       </c>
     </row>
@@ -1339,50 +1339,50 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Когда я снова стану маленьким</t>
+          <t>Город. Женитьба. Гоголь</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>24 апреля</t>
+          <t>29 апреля</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Кукольный спектакль</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>6+</t>
+          <t>12+</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Билеты</t>
+          <t>От 600 ₽</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
+          <t>Герои Гоголя растворяются в современном Петербурге</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/97786/</t>
+          <t>https://www.afisha.ru/performance/103390/</t>
         </is>
       </c>
     </row>
@@ -1392,35 +1392,35 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Что делать</t>
+          <t>Когда я снова стану маленьким</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>29 марта</t>
+          <t>24 апреля</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Кукольный спектакль</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>16+</t>
+          <t>6+</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>6.2</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>От 500 ₽</t>
+          <t>Билеты</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1430,12 +1430,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+          <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/101454/</t>
+          <t>https://www.afisha.ru/performance/97786/</t>
         </is>
       </c>
     </row>
@@ -1445,12 +1445,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Все мы прекрасные люди</t>
+          <t>Губернатор</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>19 апреля</t>
+          <t>9 апреля</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1460,35 +1460,35 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>16+</t>
+          <t>18+</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4.5</v>
+        <v>8.6</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>От 600 ₽</t>
+          <t>От 500 ₽</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/96366/</t>
+          <t>https://www.afisha.ru/performance/190192/</t>
         </is>
       </c>
     </row>
@@ -1498,12 +1498,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Губернатор</t>
+          <t>Все мы прекрасные люди</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>9 апреля</t>
+          <t>19 апреля</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1513,35 +1513,35 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>18+</t>
+          <t>16+</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>8.6</v>
+        <v>4.5</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>От 500 ₽</t>
+          <t>От 600 ₽</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
+          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/190192/</t>
+          <t>https://www.afisha.ru/performance/96366/</t>
         </is>
       </c>
     </row>
@@ -1604,12 +1604,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Трамвай «Желание»</t>
+          <t>Подыскиваю жену, недорого!</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7 апреля</t>
+          <t>16 апреля</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1628,26 +1628,26 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>7.3</v>
+        <v>5.8</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>От 1000 ₽</t>
+          <t>От 1200 ₽</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Приют комедианта</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Жестокая мелодрама с хорошими актерами</t>
+          <t>Антрепризный спектакль о превратностях любви</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/68360/</t>
+          <t>https://www.afisha.ru/performance/85589/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add column adress and duration
</commit_message>
<xml_diff>
--- a/all_performance_dict.xlsx
+++ b/all_performance_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,52 +436,62 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Название спектакля</t>
+          <t>Название</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Дата</t>
+          <t>Описание</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Время</t>
+          <t>Цена от</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Время начала</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Дата словами</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Жанр</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Возраст</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Рейтинг</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Цена</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Ссылка</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Театр</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Описание</t>
-        </is>
-      </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>URL спектакля</t>
+          <t>Возрастное ограничение</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Адрес театра</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Продолжительность</t>
         </is>
       </c>
     </row>
@@ -496,45 +506,51 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Виктор Сухоруков в трогательной комедии Вампилова</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>1 апреля</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/90900/</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>ДК им. Ленсовета</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>16+</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>ДК им. Ленсовета</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Виктор Сухоруков в трогательной комедии Вампилова</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/90900/</t>
+      <c r="L2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2 часа 40 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -549,46 +565,50 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Щекотливый спектакль без актеров и декораций</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>900</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>10 апреля</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Перформанс</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/118145/</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Скороход</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>18+</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>От 900 ₽</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Скороход</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Щекотливый спектакль без актеров и декораций</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/118145/</t>
-        </is>
+      <c r="L3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="4">
@@ -597,50 +617,56 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Смешанные чувства</t>
+          <t>Враки, или Завещание барона Мюнхгаузена</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>21 апреля</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>Константин Хабенский в роли легендарного барона</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>900</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Комедия</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>Завтра</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Премьеры</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>6.3</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>https://www.afisha.ru/performance/245895/</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/79983/</t>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>3 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -650,50 +676,58 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Враки, или Завещание барона Мюнхгаузена</t>
+          <t>Смешанные чувства</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>25 марта</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>400</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Премьеры</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>18+</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>21 апреля</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>7.2</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>https://www.afisha.ru/performance/79983/</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Константин Хабенский в роли легендарного барона</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/245895/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -703,50 +737,56 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Валентинов день</t>
+          <t>Дети солнца</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3 апреля</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>Размышления об идеальном человеке</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>400</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>23 апреля</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>От 700 ₽</t>
-        </is>
+      <c r="H6" t="n">
+        <v>5</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>https://www.afisha.ru/performance/233405/</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Иван Вырыпаев в антрепризе</t>
+          <t>Александринский театр</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/88299/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2 часа, без антракта</t>
         </is>
       </c>
     </row>
@@ -756,51 +796,55 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Иисус Христос — суперзвезда</t>
+          <t>Валентинов день</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24 апреля</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+          <t>Иван Вырыпаев в антрепризе</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>700</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Музыкальный</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>3 апреля</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/88299/</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ДК им. Ленсовета</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>12+</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>ДК им. Ленсовета</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Постановка питерского театра «Рок-опера»</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/66149/</t>
-        </is>
+      <c r="L7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="8">
@@ -809,51 +853,57 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Записки юного врача</t>
+          <t>Иисус Христос — суперзвезда</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2 апреля</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+          <t>Постановка питерского театра «Рок-о</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Драма</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>От 1200 ₽</t>
-        </is>
+          <t>24 апреля</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Музыкальный</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>8.5</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Мастерская</t>
+          <t>https://www.afisha.ru/performance/66149/</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Моноспектакль по ранним рассказам Булгакова</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117716/</t>
-        </is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Каменноостровский просп., 42</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="9">
@@ -862,51 +912,57 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ревизор</t>
+          <t>Записки юного врача</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>26 июня</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
+          <t>Моноспектакль по ранним рассказам Булгакова</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>700</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>От 400 ₽</t>
-        </is>
+          <t>2 апреля</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>7.7</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>https://www.afisha.ru/performance/117716/</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+          <t>Мастерская</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/78711/</t>
-        </is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Народная, 1</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="10">
@@ -920,45 +976,53 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>8 апреля</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/82546/</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>БДТ</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>12+</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>От 4000 ₽</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>БДТ</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/82546/</t>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 65</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3 часа, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -968,50 +1032,58 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Топливо</t>
+          <t>Все мы прекрасные люди</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>31 марта</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
+          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>600</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+          <t>19 апреля</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>4.5</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>https://www.afisha.ru/performance/96366/</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Увлекательный байопик про российского физика</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/104731/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>3 часа 20 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1021,50 +1093,58 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Гроза</t>
+          <t>Ревизор</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>28 апреля</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
+          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>400</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>8</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+          <t>26 июня</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>8.1</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>https://www.afisha.ru/performance/78711/</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Большое шаманство Андрея Могучего по Островскому</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117877/</t>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1074,50 +1154,58 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>С Чарльзом Буковски за барной стойкой</t>
+          <t>Трамвай «Желание»</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Сегодня</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+          <t>Жестокая мелодрама с хорошими актерами</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Перформанс</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>18+</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>От 900 ₽</t>
-        </is>
+          <t>7 апреля</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>7.3</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Fiddler's Green</t>
+          <t>https://www.afisha.ru/performance/68360/</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+          <t>Приют комедианта</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/191308/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Садовая, 27/9</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>3 часа 20 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1132,46 +1220,52 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>300</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>7 апреля</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>14+</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
-      </c>
       <c r="I14" t="inlineStr">
         <is>
+          <t>https://www.afisha.ru/performance/67513/</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
           <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
-        </is>
-      </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67513/</t>
-        </is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Итальянская, 19</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="15">
@@ -1180,51 +1274,55 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Дети солнца</t>
+          <t>Топливо</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>23 апреля</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
+          <t>Увлекательный байопик про российского физика</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1000</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>31 марта</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>5</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>От 300 ₽</t>
-        </is>
+      <c r="H15" t="n">
+        <v>8.4</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>https://www.afisha.ru/performance/104731/</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Размышления об идеальном человеке</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/233405/</t>
-        </is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="16">
@@ -1233,51 +1331,57 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Что делать</t>
+          <t>С Чарльзом Буковски за барной стойкой</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>29 марта</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
+          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>900</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Драма</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>От 500 ₽</t>
-        </is>
+          <t>Завтра</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Перформанс</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>5.2</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>https://www.afisha.ru/performance/191308/</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+          <t>Fiddler's Green</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/101454/</t>
-        </is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Рубинштейна, 5</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="17">
@@ -1286,50 +1390,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Преступление и наказание</t>
+          <t>Город. Женитьба. Гоголь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Герои Гоголя растворяются в современном Петербурге</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>600</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>29 апреля</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>От 1000 ₽</t>
-        </is>
+      <c r="H17" t="n">
+        <v>8.199999999999999</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Небольшой драматический театр</t>
+          <t>https://www.afisha.ru/performance/103390/</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/90576/</t>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>3 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1339,50 +1451,58 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Город. Женитьба. Гоголь</t>
+          <t>Что делать</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>29 апреля</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
+          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>500</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>29 марта</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>От 600 ₽</t>
-        </is>
+      <c r="H18" t="n">
+        <v>6.2</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>https://www.afisha.ru/performance/101454/</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Герои Гоголя растворяются в современном Петербурге</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/103390/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 65</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>1 час 35 минут, без антракта</t>
         </is>
       </c>
     </row>
@@ -1392,51 +1512,57 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Когда я снова стану маленьким</t>
+          <t>Двое в лифте не считая текилы</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>24 апреля</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
+          <t>Антреприза с Петром Красиловым и Дмитрием Орловым</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>800</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Кукольный спектакль</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6+</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Билеты</t>
-        </is>
+          <t>26 марта</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Комедия</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>6.9</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>https://www.afisha.ru/performance/93421/</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Энциклопедия подростковых грез и слез, упакованная в 15 чемоданов</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/97786/</t>
-        </is>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Каменноостровский просп., 42</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="20">
@@ -1445,50 +1571,58 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Губернатор</t>
+          <t>Гроза</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9 апреля</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
+          <t>Большое шаманство Андрея Могучего по Островскому</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>300</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>28 апреля</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>18+</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>От 500 ₽</t>
-        </is>
+      <c r="H20" t="n">
+        <v>8</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
+          <t>https://www.afisha.ru/performance/117877/</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
           <t>БДТ</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
-        </is>
-      </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/190192/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 65</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2 часа 15 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1498,51 +1632,55 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Все мы прекрасные люди</t>
+          <t>Подыскиваю жену, недорого!</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>19 апреля</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
+          <t>Антрепризный спектакль о превратностях любви</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>300</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>16 апреля</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>Комедия</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="H21" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/85589/</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>ДК им. Ленсовета</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>16+</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>От 600 ₽</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Театр им. Ленсовета</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/96366/</t>
-        </is>
+      <c r="L21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="22">
@@ -1551,50 +1689,58 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Билли Миллиган</t>
+          <t>Семья Сориано, или Итальянская комедия</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>18 апреля</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
+          <t>Знаменитый «Брак по-итальянски» в исполнении Натальи Сурковой и Сергея Барковского</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>900</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>16 апреля</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Драма</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>18+</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>От 1200 ₽</t>
-        </is>
+      <c r="H22" t="n">
+        <v>8.300000000000001</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>https://www.afisha.ru/performance/82959/</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Триллер про самого известного психа в истории</t>
+          <t>Молодежный театр на Фонтанке</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/118241/</t>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 114</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>3 часа 30 минут, 2 антракта</t>
         </is>
       </c>
     </row>
@@ -1604,50 +1750,58 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Подыскиваю жену, недорого!</t>
+          <t>Преступление и наказание</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16 апреля</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
+          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Комедия</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>29 апреля</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/90576/</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Небольшой драматический театр</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>16+</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>От 1200 ₽</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>ДК им. Ленсовета</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Антрепризный спектакль о превратностях любви</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>https://www.afisha.ru/performance/85589/</t>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>просп. КИМа, 6</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>3 часа 15 минут</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix tabe's columns: date, other dates, adress, duration. Add collections with date,rating and others.
</commit_message>
<xml_diff>
--- a/all_performance_dict.xlsx
+++ b/all_performance_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,12 +501,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Старший сын</t>
+          <t>Валентинов день</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Виктор Сухоруков в трогательной комедии Вампилова</t>
+          <t>Иван Вырыпаев в антрепризе</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1 апреля</t>
+          <t>03.04.2022</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/90900/</t>
+          <t>https://www.afisha.ru/performance/88299/</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>16+</t>
+          <t>12+</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -550,7 +550,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2 часа 40 минут, 1 антракт</t>
+          <t>2 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10 апреля</t>
+          <t>10.0422</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -607,8 +607,10 @@
       <c r="L3" t="n">
         <v>-1</v>
       </c>
-      <c r="M3" t="n">
-        <v>-1</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1 час</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -617,16 +619,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Враки, или Завещание барона Мюнхгаузена</t>
+          <t>Все мы прекрасные люди</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Константин Хабенский в роли легендарного барона</t>
+          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -635,38 +637,40 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Завтра</t>
+          <t>19.0422</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Премьеры</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/245895/</t>
+          <t>https://www.afisha.ru/performance/96366/</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>18+</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>-1</v>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Владимирский просп., 12</t>
+        </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>3 часа 30 минут, 1 антракт</t>
+          <t>3 часа 20 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -676,16 +680,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Смешанные чувства</t>
+          <t>Подыскиваю жену, недорого!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
+          <t>Антрепризный спектакль о превратностях любви</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -694,7 +698,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>21 апреля</t>
+          <t>16.0422</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -703,16 +707,16 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>7.2</v>
+        <v>5.8</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/79983/</t>
+          <t>https://www.afisha.ru/performance/85589/</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -720,14 +724,12 @@
           <t>16+</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Владимирский просп., 12</t>
-        </is>
+      <c r="L5" t="n">
+        <v>-1</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2 часа 30 минут, 1 антракт</t>
+          <t>1 час 50 минут, без антракта</t>
         </is>
       </c>
     </row>
@@ -737,16 +739,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Дети солнца</t>
+          <t>Трамвай «Желание»</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Размышления об идеальном человеке</t>
+          <t>Жестокая мелодрама с хорошими актерами</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -755,7 +757,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>23 апреля</t>
+          <t>7.0422</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -764,16 +766,16 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>7.3</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/233405/</t>
+          <t>https://www.afisha.ru/performance/68360/</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Александринский театр</t>
+          <t>Приют комедианта</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -781,12 +783,14 @@
           <t>16+</t>
         </is>
       </c>
-      <c r="L6" t="n">
-        <v>-1</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Садовая, 27/9</t>
+        </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2 часа, без антракта</t>
+          <t>3 часа 20 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -796,16 +800,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Валентинов день</t>
+          <t>Что делать</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Иван Вырыпаев в антрепризе</t>
+          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -814,7 +818,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3 апреля</t>
+          <t>02.04.2022</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -823,28 +827,32 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>7.4</v>
+        <v>6.2</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/88299/</t>
+          <t>https://www.afisha.ru/performance/101454/</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-1</v>
+          <t>16+</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 65</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1 час 35 минут, без антракта</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -853,16 +861,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Иисус Христос — суперзвезда</t>
+          <t>Смешанные чувства</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Постановка питерского театра «Рок-о</t>
+          <t>Михаил Боярский в геронтофильской комедии в компании супруги</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -871,39 +879,41 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>24 апреля</t>
+          <t>21.0422</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Музыкальный</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>8.5</v>
+        <v>7.2</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/66149/</t>
+          <t>https://www.afisha.ru/performance/79983/</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>12+</t>
+          <t>16+</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Каменноостровский просп., 42</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>-1</v>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2 часа 30 минут, 1 антракт</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -912,25 +922,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Записки юного врача</t>
+          <t>Топливо</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Моноспектакль по ранним рассказам Булгакова</t>
+          <t>Увлекательный байопик про российского физика</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2 апреля</t>
+          <t>21.0422</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -939,30 +949,30 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>7.7</v>
+        <v>8.4</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/117716/</t>
+          <t>https://www.afisha.ru/performance/104731/</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Мастерская</t>
+          <t>Скороход</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>16+</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Народная, 1</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
         <v>-1</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>1 час, без антракта</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -971,16 +981,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Лето одного года</t>
+          <t>С Чарльзом Буковски за барной стойкой</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Алиса Фрейндлих и Олег Басилашвили с блеском и мужеством играют трагикомедию о старости и об уходе вообще</t>
+          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4000</v>
+        <v>900</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -989,40 +999,40 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8 апреля</t>
+          <t>02.04.2022</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Перформанс</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>8.9</v>
+        <v>4.7</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/82546/</t>
+          <t>https://www.afisha.ru/performance/191308/</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>Fiddler's Green</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>12+</t>
+          <t>18+</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>наб. реки Фонтанки, 65</t>
+          <t>Рубинштейна, 5</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>3 часа, 1 антракт</t>
+          <t>1 час, без антракта</t>
         </is>
       </c>
     </row>
@@ -1032,16 +1042,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Все мы прекрасные люди</t>
+          <t>Записки юного врача</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Внезапная страсть героини Анны Ковальчук сокрушает ее саму и все вокруг</t>
+          <t>Моноспектакль по ранним рассказам Булгакова</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1050,25 +1060,25 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>19 апреля</t>
+          <t>02.04.2022</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/96366/</t>
+          <t>https://www.afisha.ru/performance/117716/</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>Мастерская</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1078,12 +1088,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Владимирский просп., 12</t>
+          <t>Народная, 1</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>3 часа 20 минут, 1 антракт</t>
+          <t>1 час 30 минут, без антракта</t>
         </is>
       </c>
     </row>
@@ -1093,30 +1103,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ревизор</t>
+          <t>Хулиган. Исповедь</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
+          <t>Сергей Безруков снова обращается к образу Есенина</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>26 июня</t>
+          <t>18.0522</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1124,27 +1134,25 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/78711/</t>
+          <t>https://www.afisha.ru/performance/78884/</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Театр им. Ленсовета</t>
+          <t>ДК «Выборгский»</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>12+</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Владимирский просп., 12</t>
-        </is>
+          <t>18+</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>-1</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>3 часа 30 минут, 1 антракт</t>
+          <t>2 часа, без антракта</t>
         </is>
       </c>
     </row>
@@ -1154,16 +1162,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Трамвай «Желание»</t>
+          <t>Безымянная звезда</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Жестокая мелодрама с хорошими актерами</t>
+          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1172,7 +1180,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>7 апреля</t>
+          <t>7.0422</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1181,16 +1189,16 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>7.3</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/68360/</t>
+          <t>https://www.afisha.ru/performance/67513/</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Приют комедианта</t>
+          <t>Театр им. Комиссаржевской</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1200,12 +1208,12 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Садовая, 27/9</t>
+          <t>Итальянская, 19</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>3 часа 20 минут, 1 антракт</t>
+          <t>3 часа, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1215,16 +1223,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Безымянная звезда</t>
+          <t>Мастер и Маргарита</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Первая любовь гения как неисчерпаемый источник поэзии</t>
+          <t>Screenlife-мюзикл по роману Булгакова</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1233,25 +1241,25 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>7 апреля</t>
+          <t>8.0422</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Мюзикл</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>8.199999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/67513/</t>
+          <t>https://www.afisha.ru/performance/99711/</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Театр им. Комиссаржевской</t>
+          <t>Театр ЛДМ «Новая сцена»</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1261,11 +1269,13 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Итальянская, 19</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>-1</v>
+          <t>Профессора Попова, 47</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2 часа 30 минут, 1 антракт</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1274,12 +1284,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Топливо</t>
+          <t>Иисус Христос — суперзвезда</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Увлекательный байопик про российского физика</t>
+          <t>Постановка питерского театра «Рок-опера»</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1287,30 +1297,30 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>31 марта</t>
+          <t>24.0422</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Музыкальный</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/104731/</t>
+          <t>https://www.afisha.ru/performance/66149/</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Скороход</t>
+          <t>ДК им. Ленсовета</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1318,11 +1328,15 @@
           <t>12+</t>
         </is>
       </c>
-      <c r="L15" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M15" t="n">
-        <v>-1</v>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Каменноостровский просп., 42</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2 часа, 1 антракт</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1331,16 +1345,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>С Чарльзом Буковски за барной стойкой</t>
+          <t>Губернатор</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Спектакль для одного зрителя в наушниках за барной стойкой</t>
+          <t>Зрелищный спектакль Андрея Могучего про механику тоталитаризма</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1349,25 +1363,25 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Завтра</t>
+          <t>9.0422</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Перформанс</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>5.2</v>
+        <v>8.6</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/191308/</t>
+          <t>https://www.afisha.ru/performance/190192/</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Fiddler's Green</t>
+          <t>БДТ</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1377,11 +1391,13 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Рубинштейна, 5</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>-1</v>
+          <t>наб. реки Фонтанки, 65</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>1 час 45 минут, без антракта</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1408,7 +1424,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>29 апреля</t>
+          <t>29.0422</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1417,7 +1433,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>8.199999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1451,58 +1467,58 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Что делать</t>
+          <t>Ревизор</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Разговорная антиутопия Андрея Могучего по Чернышевскому</t>
+          <t>Презабавный утренник по пьесе Гоголя, который отчего-то играют вечером</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>29 марта</t>
+          <t>26.0622</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>6.2</v>
+        <v>8.1</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/101454/</t>
+          <t>https://www.afisha.ru/performance/78711/</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>БДТ</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>16+</t>
+          <t>12+</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>наб. реки Фонтанки, 65</t>
+          <t>Владимирский просп., 12</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>1 час 35 минут, без антракта</t>
+          <t>3 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1512,16 +1528,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Двое в лифте не считая текилы</t>
+          <t>Мертвые души</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Антреприза с Петром Красиловым и Дмитрием Орловым</t>
+          <t>Спектакль-расследование от ученика Юрия Бутусова</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1530,25 +1546,25 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>26 марта</t>
+          <t>27.0422</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>6.9</v>
+        <v>6.6</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/93421/</t>
+          <t>https://www.afisha.ru/performance/207450/</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>Театр им. Ленсовета</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1558,11 +1574,13 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Каменноостровский просп., 42</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
-        <v>-1</v>
+          <t>Владимирский просп., 12</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2 часа 40 минут, 1 антракт</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1589,7 +1607,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>28 апреля</t>
+          <t>28.0422</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1632,16 +1650,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Подыскиваю жену, недорого!</t>
+          <t>Идиот. 2012</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Антрепризный спектакль о превратностях любви</t>
+          <t>Достоевский как повод порассуждать на тему «что такое хорошо и что такое плохо»</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1650,25 +1668,25 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>16 апреля</t>
+          <t>5.0422</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Комедия</t>
+          <t>Драма</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>5.8</v>
+        <v>7.2</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/85589/</t>
+          <t>https://www.afisha.ru/performance/89931/</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>ДК им. Ленсовета</t>
+          <t>Молодежный театр на Фонтанке</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1676,11 +1694,15 @@
           <t>16+</t>
         </is>
       </c>
-      <c r="L21" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M21" t="n">
-        <v>-1</v>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 114</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2 часа 50 минут, 1 антракт</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1689,25 +1711,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Семья Сориано, или Итальянская комедия</t>
+          <t>Вий</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Знаменитый «Брак по-итальянски» в исполнении Натальи Сурковой и Сергея Барковского</t>
+          <t>Нешуточный хоррор для семейного просмотра</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>16 апреля</t>
+          <t>6.0522</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1716,16 +1738,16 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/82959/</t>
+          <t>https://www.afisha.ru/performance/68503/</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Молодежный театр на Фонтанке</t>
+          <t>Большой театр кукол</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1735,12 +1757,12 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>наб. реки Фонтанки, 114</t>
+          <t>Некрасова, 10</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>3 часа 30 минут, 2 антракта</t>
+          <t>1 час 40 минут, 1 антракт</t>
         </is>
       </c>
     </row>
@@ -1750,30 +1772,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Преступление и наказание</t>
+          <t>Звездная покатуха</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Витальное прочтение студентами Льва Эренбурга одного из самых идейных текстов Достоевского</t>
+          <t>Все классические номера «Лицедеев» в одном спектакле</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>29 апреля</t>
+          <t>9.0422</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Драма</t>
+          <t>Комедия</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1781,27 +1803,88 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://www.afisha.ru/performance/90576/</t>
+          <t>https://www.afisha.ru/performance/116779/</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Небольшой драматический театр</t>
+          <t>Лицедеи</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
+          <t>12+</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Льва Толстого, 9, ТРЦ «Толстой-сквер», 4 этаж</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2 часа, 1 антракт</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Пять вечеров</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Пронзительная история о кризисе среднего возраста</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>300</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>03.04.2022</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Драма</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://www.afisha.ru/performance/68085/</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Молодежный театр на Фонтанке</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
           <t>16+</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>просп. КИМа, 6</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>3 часа 15 минут</t>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>наб. реки Фонтанки, 114</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2 часа 30 минут, 1 антракт</t>
         </is>
       </c>
     </row>

</xml_diff>